<commit_message>
Fixed empty date problem
</commit_message>
<xml_diff>
--- a/xlsx/tmp.xlsx
+++ b/xlsx/tmp.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -371,34 +371,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>44854.04166666666</v>
+        <v>44835.125</v>
       </c>
       <c r="B2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1">
-        <v>44854.08333333334</v>
-      </c>
-      <c r="B3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1">
-        <v>44854.125</v>
-      </c>
-      <c r="B4">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1">
-        <v>44854.16666666666</v>
-      </c>
-      <c r="B5">
-        <v>5.6</v>
+        <v>12.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>